<commit_message>
trying years 1-3 for aggressive
</commit_message>
<xml_diff>
--- a/mgmt/mgmt_strategies.xlsx
+++ b/mgmt/mgmt_strategies.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fossegrimen/Documents/UNH/USDA/gbPopMod/mgmt/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85FD459-D264-DB41-A8DF-679831EFF1D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27440" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27440" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -107,13 +108,13 @@
     <t>Table. Modelled management strategies on UNH woodlands. For the 12 woodland properties managed by UNH in southeasterrn New Hampshire, we simulated and compared four broad strategies for managing glossy buckthorn. These include 'No Management', where glossy buckthorn grows naturally, a 'Stated Strategy' based on the published goals for each property, a 'Management Reality' based on actions actually taken, and an 'Aggressive Strategy' with heavy manual and ground cover treatment son all properties.</t>
   </si>
   <si>
-    <t>Mechanical + chemical treatment in years 1-2 every 5 years; cover crop re-seeded after each treatment</t>
+    <t>Mechanical + chemical treatment in years 1-3 every 5 years; cover crop re-seeded after each treatment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -300,6 +301,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -567,10 +571,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -624,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -647,7 +651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -670,7 +674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -693,7 +697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -716,7 +720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -739,7 +743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -762,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -785,7 +789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -808,7 +812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -831,7 +835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="68" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
@@ -854,7 +858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" ht="68" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -877,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>

</xml_diff>